<commit_message>
Correct unit test coverage
</commit_message>
<xml_diff>
--- a/MID2025May_Database_update.xlsx
+++ b/MID2025May_Database_update.xlsx
@@ -2530,7 +2530,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0x01,0x70</t>
+          <t>0x01,0x78</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2545,7 +2545,7 @@
         <v>5.68432987514711e+23</v>
       </c>
       <c r="H28" t="n">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="I28" t="n">
         <v>25</v>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0x00,0x6E</t>
+          <t>0x00,0x6D</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3610,7 +3610,7 @@
         <v>5.68631262647113e+23</v>
       </c>
       <c r="H28" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I28" t="n">
         <v>15</v>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0x00,0x82</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -4675,7 +4675,7 @@
         <v>5.68631262647113e+23</v>
       </c>
       <c r="H28" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I28" t="n">
         <v>9</v>

</xml_diff>